<commit_message>
modified:   anuncios.xlsx deleted:    interface.py modified:   models_api/api_max.py modified:   models_api/gerar_token.py modified:   models_excel/core.py modified:   plan.xlsx modified:   teste.py new file:   view/interface.py new file:   ~$plan.xlsx
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joab.alves\Desktop\Projeto_Auto_Experts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joabe\Desktop\api_auto_experts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31195BA-5263-4D14-9F9D-FD19F5F168CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ACB8EA-049E-499D-9516-4F2BAA0CC38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5BBA7F98-EDD6-4694-9802-ACF9FB0AB750}"/>
+    <workbookView xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11175" xr2:uid="{5BBA7F98-EDD6-4694-9802-ACF9FB0AB750}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$A$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$A$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Cod Produto</t>
   </si>
@@ -63,57 +63,6 @@
   </si>
   <si>
     <t>C-1478</t>
-  </si>
-  <si>
-    <t>C-1528</t>
-  </si>
-  <si>
-    <t>C-1526</t>
-  </si>
-  <si>
-    <t>C-1500</t>
-  </si>
-  <si>
-    <t>L-663</t>
-  </si>
-  <si>
-    <t>L-733</t>
-  </si>
-  <si>
-    <t>L-533X</t>
-  </si>
-  <si>
-    <t>L-533</t>
-  </si>
-  <si>
-    <t>L-562</t>
-  </si>
-  <si>
-    <t>L-219</t>
-  </si>
-  <si>
-    <t>L-651</t>
-  </si>
-  <si>
-    <t>L-501</t>
-  </si>
-  <si>
-    <t>L-559</t>
-  </si>
-  <si>
-    <t>L-310</t>
-  </si>
-  <si>
-    <t>L-227X</t>
-  </si>
-  <si>
-    <t>L-577X</t>
-  </si>
-  <si>
-    <t>L-577</t>
-  </si>
-  <si>
-    <t>L-551</t>
   </si>
 </sst>
 </file>
@@ -491,140 +440,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CB5349-0F6B-467F-A3D7-B804A3B2BB99}">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>